<commit_message>
update WD dan Depo, langsung tanpa verifikasi
</commit_message>
<xml_diff>
--- a/public/excel/template/Template Upload Withdraw.xlsx
+++ b/public/excel/template/Template Upload Withdraw.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="120" windowWidth="13340" windowHeight="4300"/>
+    <workbookView xWindow="396" yWindow="120" windowWidth="13344" windowHeight="4296"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,21 +22,6 @@
     <t>Nama Player</t>
   </si>
   <si>
-    <t>PRO01</t>
-  </si>
-  <si>
-    <t>Player Pro 1</t>
-  </si>
-  <si>
-    <t>PRO02</t>
-  </si>
-  <si>
-    <t>Player Pro 2</t>
-  </si>
-  <si>
-    <t>2022-03-23</t>
-  </si>
-  <si>
     <t>Tanggal Withdraw</t>
   </si>
   <si>
@@ -47,6 +32,21 @@
   </si>
   <si>
     <t>Rekening Sumber Dana</t>
+  </si>
+  <si>
+    <t>angelboyx</t>
+  </si>
+  <si>
+    <t>ASEP SUPRIYADI</t>
+  </si>
+  <si>
+    <t>2022-04-24</t>
+  </si>
+  <si>
+    <t>player11</t>
+  </si>
+  <si>
+    <t>Bejo Kuncoro</t>
   </si>
 </sst>
 </file>
@@ -391,20 +391,20 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.5">
+    <row r="1" spans="1:6" ht="15.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -412,27 +412,27 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>100000</v>
@@ -441,27 +441,27 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>90000000001</v>
+        <v>12345665</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3">
-        <v>150000</v>
+        <v>15000000</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>90000000001</v>
+        <v>12345665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>